<commit_message>
updated bento tc as per bento perf data availability
</commit_message>
<xml_diff>
--- a/InputFiles/TC04_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo-TumorGrade.xlsx
+++ b/InputFiles/TC04_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo-TumorGrade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8F228E-8C99-4B7D-BCC0-500167AF8707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657683B8-783D-4317-AB0D-3CF01F14C781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="10" windowWidth="19140" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"] and d.tumor_grade In ["Intermediate Grade"]
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["standard AC followed by a taxane"] and d.tumor_grade In ["Intermediate Grade"]
 WITH ss
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)
 MATCH (s)-[:study_of_program]-&gt;(p)
@@ -90,7 +90,7 @@
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
 MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"] and d.tumor_grade In ["Intermediate Grade"]
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["standard AC followed by a taxane"] and d.tumor_grade In ["Intermediate Grade"]
 return ss.study_subject_id as `Case ID`,
        p.program_acronym as `Program Code`,
         p.program_id as Program_ID,
@@ -113,8 +113,7 @@
 MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"] and d.tumor_grade In ["Intermediate Grade"]
-WITH
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["standard AC followed by a taxane"] and d.tumor_grade In ["Intermediate Grade"]WITH
     distinct lp,
     toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
     collect(distinct f.file_id) AS files,
@@ -140,7 +139,7 @@
 MATCH (s)-[:study_of_program]-&gt;(p)
 MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
 MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
-WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"] and d.tumor_grade In ["Intermediate Grade"]
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and tp.chemotherapy_regimen In ["standard AC followed by a taxane"] and d.tumor_grade In ["Intermediate Grade"]
 RETURN  f.file_name AS `File Name`,
     head(labels(samp)) AS `Association`,
     f.file_description AS `Description`,
@@ -522,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,7 +568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>